<commit_message>
Update for spotify-high-level-dimensional-modeling #2
Update for spotify-high-level-dimensional-modeling
</commit_message>
<xml_diff>
--- a/Spotify-High-Level-Dimensional-Modeling.xlsx
+++ b/Spotify-High-Level-Dimensional-Modeling.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Perkuliahan\Semester 6\Gudang Data dan Kecerdasan Bisnis\proyek\spotify-dwbi-2022-ga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DWBI\spotify-dwbi-2022-ga\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38297D3-A9B5-42C2-92C7-EB04827B6C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>mafudge</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -133,12 +134,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>mafudge</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -154,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -167,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -180,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -193,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -206,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>Description</t>
   </si>
@@ -344,12 +345,6 @@
     <t>popularity</t>
   </si>
   <si>
-    <t>is a 36 character Universally Unique Identifier that is 
-permanently assigned to each entity in the database, i.e. 
-artists, release groups, releases, recordings, works, 
-labels, areas, places and URLs.</t>
-  </si>
-  <si>
     <t>6YjKAkDYmlasMqYw73iB0w</t>
   </si>
   <si>
@@ -359,25 +354,46 @@
     <t>Bitch Please II</t>
   </si>
   <si>
-    <t>is the total of songs in the album which will be grouped 
-based on albums consisting of one song, and albums 
-consisting of 8 or more songs</t>
-  </si>
-  <si>
     <t>album</t>
   </si>
   <si>
-    <t>at which an album or single is first offered for sale. A release
-date is sometimes called an album launch</t>
-  </si>
-  <si>
     <t>is the most heard song from the album</t>
+  </si>
+  <si>
+    <t>is a 36 character Universally Unique Identifier that is permanently assigned to each entity in the database, i.e. artists, release groups, releases, recordings, works, labels, areas, places and URLs.</t>
+  </si>
+  <si>
+    <t>is the total of songs in the album which will be grouped based on albums consisting of one song, and albums consisting of 8 or more songs</t>
+  </si>
+  <si>
+    <t>name of artist</t>
+  </si>
+  <si>
+    <t>Nancy Fletcher</t>
+  </si>
+  <si>
+    <t>unique key or primary key of artist</t>
+  </si>
+  <si>
+    <t>3E2vuvr0IQbReTbXw2MhX8</t>
+  </si>
+  <si>
+    <t>Popularity is calculated algorithmically and mostly based on the total number of plays of the track and the recency of the play.</t>
+  </si>
+  <si>
+    <t>followers</t>
+  </si>
+  <si>
+    <t>people who like or follow artist artist's profile in Spotify.</t>
+  </si>
+  <si>
+    <t>at which an album or single is first offered for sale. A release date is sometimes called an album launch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -415,13 +431,14 @@
       <name val="Inherit"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF202124"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,8 +469,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBE4D5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -477,55 +500,86 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color theme="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color theme="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color theme="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color theme="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color theme="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color theme="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -543,9 +597,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -555,23 +606,52 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1314,7 +1394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1335,7 +1415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1424,19 +1504,19 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="30">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1890,7 +1970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1898,157 +1978,175 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="33.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105.75" thickBot="1">
+    <row r="3" spans="1:5" ht="78" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A4" s="16" t="s">
-        <v>28</v>
-      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="17"/>
       <c r="B4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="60">
+      <c r="A5" s="17"/>
+      <c r="B5" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75.75" thickBot="1">
-      <c r="A5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="1:5" ht="45">
+      <c r="A6" s="17"/>
+      <c r="B6" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20">
+      <c r="C6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15">
         <v>959040000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A7" s="16" t="s">
-        <v>28</v>
-      </c>
+    <row r="7" spans="1:5">
+      <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="26" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="24"/>
+      <c r="B11" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="24"/>
+      <c r="B12" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="25">
+        <v>798</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
@@ -2408,6 +2506,10 @@
       <c r="E64" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A9:A12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update for dimension artist #2
Update for dimension artist #2
</commit_message>
<xml_diff>
--- a/Spotify-High-Level-Dimensional-Modeling.xlsx
+++ b/Spotify-High-Level-Dimensional-Modeling.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materi Kuliah\Semester 6\Gudang Data dan Kecerdasan Bisnis (DBWI)\spotify-dwbi-2022-ga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DWBI\spotify-dwbi-2022-ga\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6EB805-632F-4BD1-B4DD-18E8FBC0DB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="855" yWindow="1590" windowWidth="16065" windowHeight="9465" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>mafudge</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -133,12 +134,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>mafudge</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -154,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -167,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -180,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -193,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -206,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Description</t>
   </si>
@@ -359,27 +360,9 @@
     <t>is the total of songs in the album which will be grouped based on albums consisting of one song, and albums consisting of 8 or more songs</t>
   </si>
   <si>
-    <t>name of artist</t>
-  </si>
-  <si>
-    <t>Nancy Fletcher</t>
-  </si>
-  <si>
-    <t>unique key or primary key of artist</t>
-  </si>
-  <si>
     <t>3E2vuvr0IQbReTbXw2MhX8</t>
   </si>
   <si>
-    <t>Popularity is calculated algorithmically and mostly based on the total number of plays of the track and the recency of the play.</t>
-  </si>
-  <si>
-    <t>followers</t>
-  </si>
-  <si>
-    <t>people who like or follow artist artist's profile in Spotify.</t>
-  </si>
-  <si>
     <t>at which an album or single is first offered for sale. A release date is sometimes called an album launch</t>
   </si>
   <si>
@@ -453,12 +436,42 @@
   </si>
   <si>
     <t>merupakan nomor dari track</t>
+  </si>
+  <si>
+    <t>artist_key</t>
+  </si>
+  <si>
+    <t>kode unik sebagai primary key untuk artist</t>
+  </si>
+  <si>
+    <t>id_artist</t>
+  </si>
+  <si>
+    <t>kode unik yang mendefenisikan identitas artist</t>
+  </si>
+  <si>
+    <t>name_artist</t>
+  </si>
+  <si>
+    <t>nama artis</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>genre_artist</t>
+  </si>
+  <si>
+    <t>genre yang terkait dengan artis</t>
+  </si>
+  <si>
+    <t>hip hop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -580,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -692,81 +705,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -831,9 +775,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -870,15 +811,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,31 +820,28 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -954,7 +883,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1663,7 +1592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1684,7 +1613,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1739,7 +1668,7 @@
         <v>27</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>5</v>
@@ -1780,7 +1709,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>25</v>
@@ -2237,15 +2166,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2254,7 +2183,7 @@
     <col min="2" max="2" width="31.7109375" style="22" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" style="22" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="31" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="30" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
@@ -2281,7 +2210,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="78" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -2296,7 +2225,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="37"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="18" t="s">
         <v>30</v>
       </c>
@@ -2309,7 +2238,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="60">
-      <c r="A5" s="37"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
@@ -2322,12 +2251,12 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
-      <c r="A6" s="37"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23">
@@ -2335,7 +2264,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="38"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="18" t="s">
         <v>33</v>
       </c>
@@ -2352,482 +2281,481 @@
       <c r="B8" s="13"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="32"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="39"/>
+      <c r="E9" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="42"/>
       <c r="B10" s="14" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="39"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="42"/>
       <c r="B11" s="14" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D11" s="14"/>
-      <c r="E11" s="15">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="39"/>
+      <c r="E11" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="43"/>
       <c r="B12" s="14" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="D12" s="14"/>
-      <c r="E12" s="15">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A13" s="25"/>
+      <c r="E12" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="24"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
-      <c r="E13" s="32"/>
-    </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A14" s="40" t="s">
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="44"/>
+      <c r="B15" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="44"/>
+      <c r="B16" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="E16" s="46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17" s="44"/>
+      <c r="B17" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46">
+        <v>252746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60">
+      <c r="A18" s="44"/>
+      <c r="B18" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="46" t="s">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="44"/>
+      <c r="B19" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="52">
-        <v>252746</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A18" s="41"/>
-      <c r="B18" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="52">
+      <c r="D19" s="45"/>
+      <c r="E19" s="46">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="26"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="32"/>
+      <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="30">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <v>84231</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="43"/>
-      <c r="B22" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29">
+      <c r="A22" s="39"/>
+      <c r="B22" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28">
         <v>64021</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="44"/>
-      <c r="B23" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="34" t="s">
-        <v>63</v>
+      <c r="A23" s="40"/>
+      <c r="B23" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="25"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="35"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="34"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="35"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="35"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="35"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="35"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="34"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="35"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="34"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="35"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="35"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="35"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="35"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="35"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="35"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="34"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="35"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="34"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="35"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="35"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="35"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="35"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="34"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="35"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="34"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="35"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="34"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="35"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="35"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="35"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="35"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="35"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="35"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="35"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="34"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="35"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="34"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="35"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="35"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="35"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="35"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="35"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="27"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="35"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="35"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="27"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="35"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="35"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="35"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="35"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="34"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="27"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="35"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="34"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="27"/>
+      <c r="A63" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A9:A12"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A21:A23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1"/>
+    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>